<commit_message>
fix to cleaning data
</commit_message>
<xml_diff>
--- a/trading_legend.xlsx
+++ b/trading_legend.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y89"/>
+  <dimension ref="A1:Y96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1004,7 +1004,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>S, SSR</t>
+          <t>S</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>S, SSR</t>
+          <t>S</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -4085,7 +4085,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>SR, SSR, UR</t>
+          <t>SR</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -5832,7 +5832,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>SR, SSR</t>
+          <t>SR</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -6667,7 +6667,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>SR, SSR, UR</t>
+          <t>SR</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -7388,6 +7388,523 @@
           <t>World Conqueror: This Retainer Earnings +5%</t>
         </is>
       </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>SSR</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Wu Shiren</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Rover</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Status Level 9</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>36</v>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Ordinary Aptitude: Aptitude +1</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Art of Chivalry: Aptitude +1</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>Retainer Deployment: When deployed, building earnings +30%</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>Business: Aptitude +1</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr"/>
+      <c r="L90" t="inlineStr"/>
+      <c r="M90" t="inlineStr"/>
+      <c r="N90" t="inlineStr"/>
+      <c r="O90" t="inlineStr"/>
+      <c r="P90" t="inlineStr"/>
+      <c r="Q90" t="inlineStr"/>
+      <c r="R90" t="inlineStr"/>
+      <c r="S90" t="inlineStr"/>
+      <c r="T90" t="inlineStr"/>
+      <c r="U90" t="inlineStr"/>
+      <c r="V90" t="inlineStr"/>
+      <c r="W90" t="inlineStr"/>
+      <c r="X90" t="inlineStr"/>
+      <c r="Y90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>SSR</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Cook Zheng</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Artisan</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Status Level 13</t>
+        </is>
+      </c>
+      <c r="F91" t="n">
+        <v>36</v>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Ordinary Aptitude: Aptitude +1</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Art of Ingenuity: Aptitude +1</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>Retainer Deployment: When deployed, building earnings +30%</t>
+        </is>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>Business: Aptitude +1</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr"/>
+      <c r="L91" t="inlineStr"/>
+      <c r="M91" t="inlineStr"/>
+      <c r="N91" t="inlineStr"/>
+      <c r="O91" t="inlineStr"/>
+      <c r="P91" t="inlineStr"/>
+      <c r="Q91" t="inlineStr"/>
+      <c r="R91" t="inlineStr"/>
+      <c r="S91" t="inlineStr"/>
+      <c r="T91" t="inlineStr"/>
+      <c r="U91" t="inlineStr"/>
+      <c r="V91" t="inlineStr"/>
+      <c r="W91" t="inlineStr"/>
+      <c r="X91" t="inlineStr"/>
+      <c r="Y91" t="inlineStr"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>SSR</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Calabash Immortal</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Merchant</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Bandits Den</t>
+        </is>
+      </c>
+      <c r="F92" t="n">
+        <v>55</v>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Good Aptitude: Aptitude +2</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Art of Business: Aptitude +1</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>Retainer Deployment: When deployed, building earnings +30%</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>Business: Aptitude +1</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr"/>
+      <c r="L92" t="inlineStr"/>
+      <c r="M92" t="inlineStr"/>
+      <c r="N92" t="inlineStr"/>
+      <c r="O92" t="inlineStr"/>
+      <c r="P92" t="inlineStr"/>
+      <c r="Q92" t="inlineStr"/>
+      <c r="R92" t="inlineStr"/>
+      <c r="S92" t="inlineStr">
+        <is>
+          <t>Big Profit: Earnings of Merchant Retainer +5% in Trade War and Saltern battles</t>
+        </is>
+      </c>
+      <c r="T92" t="inlineStr"/>
+      <c r="U92" t="inlineStr"/>
+      <c r="V92" t="inlineStr"/>
+      <c r="W92" t="inlineStr"/>
+      <c r="X92" t="inlineStr"/>
+      <c r="Y92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>UR</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Calabash Immortal</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Merchant</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Bandits Den</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>55</v>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Good Aptitude: Aptitude +2</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>Art of Business: Aptitude +1</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>Retainer Deployment: When deployed, building earnings +30%</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>Business: Aptitude +1</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr"/>
+      <c r="L93" t="inlineStr"/>
+      <c r="M93" t="inlineStr"/>
+      <c r="N93" t="inlineStr"/>
+      <c r="O93" t="inlineStr"/>
+      <c r="P93" t="inlineStr"/>
+      <c r="Q93" t="inlineStr"/>
+      <c r="R93" t="inlineStr"/>
+      <c r="S93" t="inlineStr">
+        <is>
+          <t>Big Profit: Earnings of Merchant Retainer +5% in Trade War and Saltern battles</t>
+        </is>
+      </c>
+      <c r="T93" t="inlineStr"/>
+      <c r="U93" t="inlineStr"/>
+      <c r="V93" t="inlineStr"/>
+      <c r="W93" t="inlineStr"/>
+      <c r="X93" t="inlineStr"/>
+      <c r="Y93" t="inlineStr"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>SSR</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Xie Lu</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Scholar</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Chef Contest</t>
+        </is>
+      </c>
+      <c r="F94" t="n">
+        <v>55</v>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Good Aptitude: Aptitude +2</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Art of Scholarship: Aptitude +1</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>Retainer Deployment: When deployed, building earnings +30%</t>
+        </is>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>Business: Aptitude +1</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr"/>
+      <c r="L94" t="inlineStr"/>
+      <c r="M94" t="inlineStr"/>
+      <c r="N94" t="inlineStr"/>
+      <c r="O94" t="inlineStr"/>
+      <c r="P94" t="inlineStr"/>
+      <c r="Q94" t="inlineStr"/>
+      <c r="R94" t="inlineStr"/>
+      <c r="S94" t="inlineStr">
+        <is>
+          <t>Big Profit: Earnings of Scholar Retainer +5% in Trade War and Saltern battles</t>
+        </is>
+      </c>
+      <c r="T94" t="inlineStr"/>
+      <c r="U94" t="inlineStr"/>
+      <c r="V94" t="inlineStr"/>
+      <c r="W94" t="inlineStr">
+        <is>
+          <t>Ace Cook: Earnings +5% (For each ace cook recruited, earnings +5%)</t>
+        </is>
+      </c>
+      <c r="X94" t="inlineStr">
+        <is>
+          <t>True Cooking Master Boy: Earnings +5%</t>
+        </is>
+      </c>
+      <c r="Y94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>SSR</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Tang San</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Peasant</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Soul Land</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>55</v>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Good Aptitude: Aptitude +2</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>Art of Farming: Aptitude +1</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>Retainer Deployment: When deployed, building earnings +30%</t>
+        </is>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>Business: Aptitude +1</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>Resilient Grass: Aptitude +3</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>Spider Lances: Aptitude +3</t>
+        </is>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>Incarnation of Haitian: Aptitude +4</t>
+        </is>
+      </c>
+      <c r="N95" t="inlineStr">
+        <is>
+          <t>Ult Art of Farming: Aptitude +3</t>
+        </is>
+      </c>
+      <c r="O95" t="inlineStr"/>
+      <c r="P95" t="inlineStr"/>
+      <c r="Q95" t="inlineStr"/>
+      <c r="R95" t="inlineStr"/>
+      <c r="S95" t="inlineStr">
+        <is>
+          <t>Prosperity: Earnings of Peasant Retainer +20% in Trade War and Saltern battles</t>
+        </is>
+      </c>
+      <c r="T95" t="inlineStr">
+        <is>
+          <t>Fortunate Farmer: Earnings of all peasant retainers +5%</t>
+        </is>
+      </c>
+      <c r="U95" t="inlineStr">
+        <is>
+          <t>Master of Tang Sect: Beauty Charm +10% when deployed to Bazaar Palace</t>
+        </is>
+      </c>
+      <c r="V95" t="inlineStr"/>
+      <c r="W95" t="inlineStr"/>
+      <c r="X95" t="inlineStr"/>
+      <c r="Y95" t="inlineStr"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>UR</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Tang San</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Peasant</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Soul Land</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
+        <v>55</v>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Good Aptitude: Aptitude +2</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>Art of Farming: Aptitude +1</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>Retainer Deployment: When deployed, building earnings +30%</t>
+        </is>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>Business: Aptitude +1</t>
+        </is>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>Resilient Grass: Aptitude +3</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>Spider Lances: Aptitude +3</t>
+        </is>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>Incarnation of Haitian: Aptitude +4</t>
+        </is>
+      </c>
+      <c r="N96" t="inlineStr">
+        <is>
+          <t>Ult Art of Farming: Aptitude +3</t>
+        </is>
+      </c>
+      <c r="O96" t="inlineStr"/>
+      <c r="P96" t="inlineStr"/>
+      <c r="Q96" t="inlineStr"/>
+      <c r="R96" t="inlineStr"/>
+      <c r="S96" t="inlineStr">
+        <is>
+          <t>Prosperity: Earnings of Peasant Retainer +20% in Trade War and Saltern battles</t>
+        </is>
+      </c>
+      <c r="T96" t="inlineStr">
+        <is>
+          <t>Fortunate Farmer: Earnings of all peasant retainers +5%</t>
+        </is>
+      </c>
+      <c r="U96" t="inlineStr">
+        <is>
+          <t>Master of Tang Sect: Beauty Charm +10% when deployed to Bazaar Palace</t>
+        </is>
+      </c>
+      <c r="V96" t="inlineStr"/>
+      <c r="W96" t="inlineStr"/>
+      <c r="X96" t="inlineStr"/>
+      <c r="Y96" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>